<commit_message>
set up grading system
</commit_message>
<xml_diff>
--- a/201-8 (W25)/grades/000 template.xlsx
+++ b/201-8 (W25)/grades/000 template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlatza\Documents\winter2025\201-8 (W25)\grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA06660-DB3B-4F93-9ADB-8030BE97C901}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90835BA1-451D-46E4-A3D9-95F0687A702D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{380839EA-A048-45B5-9384-B1EC17772E6F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="44">
   <si>
     <t>PH201-8 quiz 1</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>q-value</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -507,19 +510,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -568,36 +558,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -649,36 +609,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -732,6 +662,43 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -739,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -756,11 +723,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -773,21 +740,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -799,143 +764,158 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1252,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964C4774-8121-4B0E-85A4-DEE73D585D3B}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:H18"/>
+      <selection activeCell="F17" sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1519,23 +1499,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1544,58 +1524,58 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="61" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="63" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="64"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="9">
         <v>1</v>
       </c>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="65" t="s">
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="66"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="7">
         <v>3</v>
       </c>
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="57"/>
-      <c r="B7" s="58"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1608,17 +1588,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="79" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="44"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="15">
         <v>1</v>
       </c>
@@ -1627,15 +1607,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="41"/>
-      <c r="B9" s="45" t="s">
+    <row r="9" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="80"/>
+      <c r="B9" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="59"/>
       <c r="E9" s="17">
         <v>2</v>
       </c>
@@ -1644,13 +1624,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46" t="s">
+    <row r="10" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="80"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="19">
         <v>4</v>
       </c>
@@ -1660,165 +1640,210 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="33" t="s">
+      <c r="A11" s="80"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="17">
         <v>4</v>
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="41"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46" t="s">
+    <row r="12" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="80"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="47"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="19">
         <v>1</v>
       </c>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
-      <c r="B13" s="45" t="s">
+    <row r="13" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="80"/>
+      <c r="B13" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="17">
         <v>2</v>
       </c>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="46" t="s">
+    <row r="14" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="80"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="47"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="19">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="41"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="33" t="s">
+      <c r="A15" s="80"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="59"/>
       <c r="E15" s="17">
         <v>4</v>
       </c>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="42"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="35" t="s">
+    <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="80"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="61"/>
       <c r="E16" s="21">
         <v>1</v>
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="37" t="s">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="80"/>
+      <c r="B17" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="23">
+      <c r="C17" s="77"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="71">
         <f>SUM(E3:E16)</f>
         <v>30</v>
       </c>
-      <c r="F17" s="24">
-        <f>SUM(F3:F16)</f>
+      <c r="F17" s="72">
+        <f>SUM(F3:F16,F18:F21)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="72" t="s">
+      <c r="L17" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="80"/>
+      <c r="B18" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="30"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="74" t="s">
+      <c r="E18" s="74">
+        <v>2</v>
+      </c>
+      <c r="F18" s="74"/>
+      <c r="I18" s="28"/>
+      <c r="L18" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="80"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="75" t="s">
+        <v>19</v>
+      </c>
       <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="32"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="76" t="s">
+      <c r="E19" s="9">
+        <v>4</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="I19" s="30"/>
+      <c r="L19" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="31"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="80"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="74">
+        <v>4</v>
+      </c>
+      <c r="F20" s="74"/>
+      <c r="I20" s="29"/>
+      <c r="L20" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="80"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="75"/>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="I21" s="29"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="C14:D14"/>
+  <mergeCells count="29">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A8:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:B7"/>
@@ -1826,10 +1851,13 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="M17:S17"/>
+    <mergeCell ref="M18:S18"/>
+    <mergeCell ref="M19:S19"/>
+    <mergeCell ref="M20:S20"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A8:A16"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:D9"/>
@@ -1837,7 +1865,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1859,686 +1886,696 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="70"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="29">
+      <c r="B4" s="67"/>
+      <c r="C4" s="27">
         <v>3</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="29">
+      <c r="B5" s="67"/>
+      <c r="C5" s="27">
         <v>6</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="29">
-        <v>4</v>
-      </c>
-      <c r="D6" s="29"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="27">
+        <v>4</v>
+      </c>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="29">
+      <c r="B7" s="67"/>
+      <c r="C7" s="27">
         <v>1</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="29">
+      <c r="B8" s="67"/>
+      <c r="C8" s="27">
         <v>3</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="29">
-        <v>4</v>
-      </c>
-      <c r="D9" s="29"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="27">
+        <v>4</v>
+      </c>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="27"/>
-      <c r="B11" s="29" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="27">
         <v>2</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="29">
-        <v>4</v>
-      </c>
-      <c r="D12" s="29"/>
+      <c r="C12" s="27">
+        <v>4</v>
+      </c>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="27"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="29">
-        <v>4</v>
-      </c>
-      <c r="D13" s="29"/>
+      <c r="C13" s="27">
+        <v>4</v>
+      </c>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="27"/>
-      <c r="B14" s="29" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="27">
         <v>1</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="68"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="27"/>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="27">
         <v>2</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="27"/>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="29">
-        <v>4</v>
-      </c>
-      <c r="D17" s="29"/>
+      <c r="C17" s="27">
+        <v>4</v>
+      </c>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="29">
-        <v>4</v>
-      </c>
-      <c r="D18" s="29"/>
+      <c r="C18" s="27">
+        <v>4</v>
+      </c>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
-      <c r="B19" s="29" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="27">
         <v>1</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="29">
+      <c r="B20" s="67"/>
+      <c r="C20" s="27">
         <v>2</v>
       </c>
-      <c r="D20" s="29"/>
+      <c r="D20" s="27"/>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="29" t="s">
+      <c r="A21" s="25"/>
+      <c r="B21" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="27">
         <v>45</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="69"/>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="71"/>
+      <c r="A22" s="68"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="70"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="67" t="s">
+      <c r="A23" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="68"/>
-      <c r="C23" s="29">
+      <c r="B23" s="67"/>
+      <c r="C23" s="27">
         <v>1</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="27"/>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="29">
+      <c r="B24" s="67"/>
+      <c r="C24" s="27">
         <v>3</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="27"/>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="67" t="s">
+      <c r="A25" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="68"/>
-      <c r="C25" s="29">
+      <c r="B25" s="67"/>
+      <c r="C25" s="27">
         <v>6</v>
       </c>
-      <c r="D25" s="29"/>
+      <c r="D25" s="27"/>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="29">
-        <v>4</v>
-      </c>
-      <c r="D26" s="29"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="27">
+        <v>4</v>
+      </c>
+      <c r="D26" s="27"/>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="67" t="s">
+      <c r="A27" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="29">
+      <c r="B27" s="67"/>
+      <c r="C27" s="27">
         <v>1</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="27"/>
     </row>
     <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="29">
+      <c r="B28" s="67"/>
+      <c r="C28" s="27">
         <v>3</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="27"/>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="67" t="s">
+      <c r="A29" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="68"/>
-      <c r="C29" s="29">
-        <v>4</v>
-      </c>
-      <c r="D29" s="29"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="27">
+        <v>4</v>
+      </c>
+      <c r="D29" s="27"/>
     </row>
     <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="27"/>
-      <c r="B30" s="29" t="s">
+      <c r="A30" s="25"/>
+      <c r="B30" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="29">
+      <c r="C30" s="27">
         <v>2</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="27"/>
-      <c r="B31" s="29" t="s">
+      <c r="A31" s="25"/>
+      <c r="B31" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="29">
-        <v>4</v>
-      </c>
-      <c r="D31" s="29"/>
+      <c r="C31" s="27">
+        <v>4</v>
+      </c>
+      <c r="D31" s="27"/>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="27"/>
-      <c r="B32" s="29" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="29">
-        <v>4</v>
-      </c>
-      <c r="D32" s="29"/>
+      <c r="C32" s="27">
+        <v>4</v>
+      </c>
+      <c r="D32" s="27"/>
     </row>
     <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="27"/>
-      <c r="B33" s="29" t="s">
+      <c r="A33" s="25"/>
+      <c r="B33" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="29">
+      <c r="C33" s="27">
         <v>1</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="27"/>
     </row>
     <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
     </row>
     <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="27"/>
-      <c r="B35" s="29" t="s">
+      <c r="A35" s="25"/>
+      <c r="B35" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="29">
+      <c r="C35" s="27">
         <v>2</v>
       </c>
-      <c r="D35" s="29"/>
+      <c r="D35" s="27"/>
     </row>
     <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="27"/>
-      <c r="B36" s="29" t="s">
+      <c r="A36" s="25"/>
+      <c r="B36" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="29">
-        <v>4</v>
-      </c>
-      <c r="D36" s="29"/>
+      <c r="C36" s="27">
+        <v>4</v>
+      </c>
+      <c r="D36" s="27"/>
     </row>
     <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="27"/>
-      <c r="B37" s="29" t="s">
+      <c r="A37" s="25"/>
+      <c r="B37" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="29">
-        <v>4</v>
-      </c>
-      <c r="D37" s="29"/>
+      <c r="C37" s="27">
+        <v>4</v>
+      </c>
+      <c r="D37" s="27"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="27"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="25"/>
+      <c r="B38" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38" s="27">
         <v>1</v>
       </c>
-      <c r="D38" s="29"/>
+      <c r="D38" s="27"/>
     </row>
     <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="67" t="s">
+      <c r="A39" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="68"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
     </row>
     <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="27"/>
-      <c r="B40" s="29" t="s">
+      <c r="A40" s="25"/>
+      <c r="B40" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="29">
+      <c r="C40" s="27">
         <v>2</v>
       </c>
-      <c r="D40" s="29"/>
+      <c r="D40" s="27"/>
     </row>
     <row r="41" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="27"/>
-      <c r="B41" s="29" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="29">
-        <v>4</v>
-      </c>
-      <c r="D41" s="29"/>
+      <c r="C41" s="27">
+        <v>4</v>
+      </c>
+      <c r="D41" s="27"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="27"/>
-      <c r="B42" s="29" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="29">
-        <v>4</v>
-      </c>
-      <c r="D42" s="29"/>
+      <c r="C42" s="27">
+        <v>4</v>
+      </c>
+      <c r="D42" s="27"/>
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="27"/>
-      <c r="B43" s="29" t="s">
+      <c r="A43" s="25"/>
+      <c r="B43" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="29">
+      <c r="C43" s="27">
         <v>1</v>
       </c>
-      <c r="D43" s="29"/>
+      <c r="D43" s="27"/>
     </row>
     <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="29">
+      <c r="B44" s="67"/>
+      <c r="C44" s="27">
         <v>5</v>
       </c>
-      <c r="D44" s="29"/>
+      <c r="D44" s="27"/>
     </row>
     <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="27"/>
-      <c r="B45" s="29" t="s">
+      <c r="A45" s="25"/>
+      <c r="B45" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="29">
+      <c r="C45" s="27">
         <v>60</v>
       </c>
-      <c r="D45" s="29"/>
+      <c r="D45" s="27"/>
     </row>
     <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="69"/>
-      <c r="B46" s="70"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="71"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="70"/>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="67" t="s">
+      <c r="A47" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="68"/>
-      <c r="C47" s="29">
+      <c r="B47" s="67"/>
+      <c r="C47" s="27">
         <v>1</v>
       </c>
-      <c r="D47" s="29"/>
+      <c r="D47" s="27"/>
     </row>
     <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="67" t="s">
+      <c r="A48" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="68"/>
-      <c r="C48" s="29">
+      <c r="B48" s="67"/>
+      <c r="C48" s="27">
         <v>3</v>
       </c>
-      <c r="D48" s="29"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="67" t="s">
+      <c r="A49" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="68"/>
-      <c r="C49" s="29">
+      <c r="B49" s="67"/>
+      <c r="C49" s="27">
         <v>6</v>
       </c>
-      <c r="D49" s="29"/>
+      <c r="D49" s="27"/>
     </row>
     <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="67" t="s">
+      <c r="A50" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="68"/>
-      <c r="C50" s="29">
-        <v>4</v>
-      </c>
-      <c r="D50" s="29"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="27">
+        <v>4</v>
+      </c>
+      <c r="D50" s="27"/>
     </row>
     <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="67" t="s">
+      <c r="A51" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="68"/>
-      <c r="C51" s="29">
+      <c r="B51" s="67"/>
+      <c r="C51" s="27">
         <v>1</v>
       </c>
-      <c r="D51" s="29"/>
+      <c r="D51" s="27"/>
     </row>
     <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="67" t="s">
+      <c r="A52" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="68"/>
-      <c r="C52" s="29">
+      <c r="B52" s="67"/>
+      <c r="C52" s="27">
         <v>3</v>
       </c>
-      <c r="D52" s="29"/>
+      <c r="D52" s="27"/>
     </row>
     <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="67" t="s">
+      <c r="A53" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="68"/>
-      <c r="C53" s="29">
-        <v>4</v>
-      </c>
-      <c r="D53" s="29"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="27">
+        <v>4</v>
+      </c>
+      <c r="D53" s="27"/>
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="27"/>
-      <c r="B54" s="29" t="s">
+      <c r="A54" s="25"/>
+      <c r="B54" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="29">
+      <c r="C54" s="27">
         <v>2</v>
       </c>
-      <c r="D54" s="29"/>
+      <c r="D54" s="27"/>
     </row>
     <row r="55" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="27"/>
-      <c r="B55" s="29" t="s">
+      <c r="A55" s="25"/>
+      <c r="B55" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="29">
-        <v>4</v>
-      </c>
-      <c r="D55" s="29"/>
+      <c r="C55" s="27">
+        <v>4</v>
+      </c>
+      <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="27"/>
-      <c r="B56" s="29" t="s">
+      <c r="A56" s="25"/>
+      <c r="B56" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C56" s="29">
-        <v>4</v>
-      </c>
-      <c r="D56" s="29"/>
+      <c r="C56" s="27">
+        <v>4</v>
+      </c>
+      <c r="D56" s="27"/>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="27"/>
-      <c r="B57" s="29" t="s">
+      <c r="A57" s="25"/>
+      <c r="B57" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="29">
+      <c r="C57" s="27">
         <v>1</v>
       </c>
-      <c r="D57" s="29"/>
+      <c r="D57" s="27"/>
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="67" t="s">
+      <c r="A58" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="68"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
+      <c r="B58" s="67"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="27"/>
-      <c r="B59" s="29" t="s">
+      <c r="A59" s="25"/>
+      <c r="B59" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="29">
+      <c r="C59" s="27">
         <v>2</v>
       </c>
-      <c r="D59" s="29"/>
+      <c r="D59" s="27"/>
     </row>
     <row r="60" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="27"/>
-      <c r="B60" s="29" t="s">
+      <c r="A60" s="25"/>
+      <c r="B60" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="29">
-        <v>4</v>
-      </c>
-      <c r="D60" s="29"/>
+      <c r="C60" s="27">
+        <v>4</v>
+      </c>
+      <c r="D60" s="27"/>
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="27"/>
-      <c r="B61" s="29" t="s">
+      <c r="A61" s="25"/>
+      <c r="B61" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="29">
-        <v>4</v>
-      </c>
-      <c r="D61" s="29"/>
+      <c r="C61" s="27">
+        <v>4</v>
+      </c>
+      <c r="D61" s="27"/>
     </row>
     <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="27"/>
-      <c r="B62" s="29" t="s">
+      <c r="A62" s="25"/>
+      <c r="B62" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="29">
+      <c r="C62" s="27">
         <v>1</v>
       </c>
-      <c r="D62" s="29"/>
+      <c r="D62" s="27"/>
     </row>
     <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="67" t="s">
+      <c r="A63" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B63" s="68"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
+      <c r="B63" s="67"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="27"/>
-      <c r="B64" s="29" t="s">
+      <c r="A64" s="25"/>
+      <c r="B64" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C64" s="29">
+      <c r="C64" s="27">
         <v>2</v>
       </c>
-      <c r="D64" s="29"/>
+      <c r="D64" s="27"/>
     </row>
     <row r="65" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="27"/>
-      <c r="B65" s="29" t="s">
+      <c r="A65" s="25"/>
+      <c r="B65" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C65" s="29">
-        <v>4</v>
-      </c>
-      <c r="D65" s="29"/>
+      <c r="C65" s="27">
+        <v>4</v>
+      </c>
+      <c r="D65" s="27"/>
     </row>
     <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="27"/>
-      <c r="B66" s="29" t="s">
+      <c r="A66" s="25"/>
+      <c r="B66" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="29">
-        <v>4</v>
-      </c>
-      <c r="D66" s="29"/>
+      <c r="C66" s="27">
+        <v>4</v>
+      </c>
+      <c r="D66" s="27"/>
     </row>
     <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="27"/>
-      <c r="B67" s="29" t="s">
+      <c r="A67" s="25"/>
+      <c r="B67" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="29">
+      <c r="C67" s="27">
         <v>1</v>
       </c>
-      <c r="D67" s="29"/>
+      <c r="D67" s="27"/>
     </row>
     <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="67" t="s">
+      <c r="A68" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B68" s="68"/>
-      <c r="C68" s="29">
+      <c r="B68" s="67"/>
+      <c r="C68" s="27">
         <v>5</v>
       </c>
-      <c r="D68" s="29"/>
+      <c r="D68" s="27"/>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="27"/>
-      <c r="B69" s="29" t="s">
+      <c r="A69" s="25"/>
+      <c r="B69" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C69" s="29">
+      <c r="C69" s="27">
         <v>60</v>
       </c>
-      <c r="D69" s="29"/>
+      <c r="D69" s="27"/>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="67" t="s">
+      <c r="A70" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="B70" s="68"/>
-      <c r="C70" s="29">
+      <c r="B70" s="67"/>
+      <c r="C70" s="27">
         <v>185</v>
       </c>
-      <c r="D70" s="29"/>
+      <c r="D70" s="27"/>
     </row>
     <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="67"/>
-      <c r="B71" s="68"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="29"/>
+      <c r="A71" s="66"/>
+      <c r="B71" s="67"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A8:B8"/>
@@ -2554,21 +2591,11 @@
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>